<commit_message>
Default Log Path Fixed.
</commit_message>
<xml_diff>
--- a/Termie/bin/Debug.xlsx
+++ b/Termie/bin/Debug.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="192" yWindow="108" windowWidth="16776" windowHeight="7752"/>
+    <workbookView xWindow="480" yWindow="84" windowWidth="22056" windowHeight="11424"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
-    <t>Time(sec)</t>
+    <t>Time</t>
   </si>
   <si>
     <t>Breath</t>
@@ -381,7 +381,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E12"/>
+  <dimension ref="A1:E18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -406,13 +406,13 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A2">
-        <v>3.04</v>
+        <v>12.327</v>
       </c>
       <c r="B2">
         <v>-1.6599999740719795E-2</v>
       </c>
       <c r="C2">
-        <v>10943.6025390625</v>
+        <v>10998.64453125</v>
       </c>
       <c r="D2">
         <v>120</v>
@@ -423,13 +423,13 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A3">
-        <v>3.3</v>
+        <v>12.586</v>
       </c>
       <c r="B3">
         <v>-1.6599999740719795E-2</v>
       </c>
       <c r="C3">
-        <v>10943.6650390625</v>
+        <v>10998.6728515625</v>
       </c>
       <c r="D3">
         <v>120</v>
@@ -440,81 +440,81 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A4">
-        <v>3.55</v>
+        <v>12.843999999999999</v>
       </c>
       <c r="B4">
         <v>-1.6599999740719795E-2</v>
       </c>
       <c r="C4">
-        <v>10943.572265625</v>
+        <v>10998.5966796875</v>
       </c>
       <c r="D4">
-        <v>90</v>
+        <v>120</v>
       </c>
       <c r="E4">
-        <v>90</v>
+        <v>120</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A5">
-        <v>3.81</v>
+        <v>13.103</v>
       </c>
       <c r="B5">
         <v>-1.6599999740719795E-2</v>
       </c>
       <c r="C5">
-        <v>10943.51171875</v>
+        <v>10998.7626953125</v>
       </c>
       <c r="D5">
-        <v>90</v>
+        <v>120</v>
       </c>
       <c r="E5">
-        <v>90</v>
+        <v>120</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A6">
-        <v>4.07</v>
+        <v>13.361000000000001</v>
       </c>
       <c r="B6">
         <v>-1.6599999740719795E-2</v>
       </c>
       <c r="C6">
-        <v>10943.5654296875</v>
+        <v>10998.654296875</v>
       </c>
       <c r="D6">
-        <v>90</v>
+        <v>120</v>
       </c>
       <c r="E6">
-        <v>90</v>
+        <v>120</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A7">
-        <v>4.33</v>
+        <v>13.62</v>
       </c>
       <c r="B7">
         <v>-1.6599999740719795E-2</v>
       </c>
       <c r="C7">
-        <v>10943.51171875</v>
+        <v>10998.646484375</v>
       </c>
       <c r="D7">
-        <v>90</v>
+        <v>120</v>
       </c>
       <c r="E7">
-        <v>90</v>
+        <v>120</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A8">
-        <v>4.59</v>
+        <v>13.879</v>
       </c>
       <c r="B8">
         <v>-1.6599999740719795E-2</v>
       </c>
       <c r="C8">
-        <v>10943.513671875</v>
+        <v>10998.6025390625</v>
       </c>
       <c r="D8">
         <v>120</v>
@@ -525,13 +525,13 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A9">
-        <v>4.8499999999999996</v>
+        <v>14.137</v>
       </c>
       <c r="B9">
         <v>-1.6599999740719795E-2</v>
       </c>
       <c r="C9">
-        <v>10943.4345703125</v>
+        <v>10998.6123046875</v>
       </c>
       <c r="D9">
         <v>120</v>
@@ -542,13 +542,13 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A10">
-        <v>5.0999999999999996</v>
+        <v>14.396000000000001</v>
       </c>
       <c r="B10">
         <v>-1.6599999740719795E-2</v>
       </c>
       <c r="C10">
-        <v>10943.4580078125</v>
+        <v>10998.640625</v>
       </c>
       <c r="D10">
         <v>120</v>
@@ -559,13 +559,13 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A11">
-        <v>5.36</v>
+        <v>14.654</v>
       </c>
       <c r="B11">
         <v>-1.6599999740719795E-2</v>
       </c>
       <c r="C11">
-        <v>10943.5263671875</v>
+        <v>10998.673828125</v>
       </c>
       <c r="D11">
         <v>120</v>
@@ -576,18 +576,120 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A12">
-        <v>5.62</v>
+        <v>14.913</v>
       </c>
       <c r="B12">
         <v>-1.6599999740719795E-2</v>
       </c>
       <c r="C12">
-        <v>10943.5478515625</v>
+        <v>10998.5576171875</v>
       </c>
       <c r="D12">
         <v>120</v>
       </c>
       <c r="E12">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A13">
+        <v>15.170999999999999</v>
+      </c>
+      <c r="B13">
+        <v>-1.6599999740719795E-2</v>
+      </c>
+      <c r="C13">
+        <v>10998.5693359375</v>
+      </c>
+      <c r="D13">
+        <v>120</v>
+      </c>
+      <c r="E13">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A14">
+        <v>15.43</v>
+      </c>
+      <c r="B14">
+        <v>-1.6599999740719795E-2</v>
+      </c>
+      <c r="C14">
+        <v>10998.640625</v>
+      </c>
+      <c r="D14">
+        <v>120</v>
+      </c>
+      <c r="E14">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A15">
+        <v>15.689</v>
+      </c>
+      <c r="B15">
+        <v>-1.6599999740719795E-2</v>
+      </c>
+      <c r="C15">
+        <v>10998.6142578125</v>
+      </c>
+      <c r="D15">
+        <v>120</v>
+      </c>
+      <c r="E15">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A16">
+        <v>15.946999999999999</v>
+      </c>
+      <c r="B16">
+        <v>-1.6599999740719795E-2</v>
+      </c>
+      <c r="C16">
+        <v>10998.576171875</v>
+      </c>
+      <c r="D16">
+        <v>120</v>
+      </c>
+      <c r="E16">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A17">
+        <v>16.206</v>
+      </c>
+      <c r="B17">
+        <v>-1.6599999740719795E-2</v>
+      </c>
+      <c r="C17">
+        <v>10998.5732421875</v>
+      </c>
+      <c r="D17">
+        <v>120</v>
+      </c>
+      <c r="E17">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A18">
+        <v>16.463999999999999</v>
+      </c>
+      <c r="B18">
+        <v>-1.6599999740719795E-2</v>
+      </c>
+      <c r="C18">
+        <v>10998.5048828125</v>
+      </c>
+      <c r="D18">
+        <v>120</v>
+      </c>
+      <c r="E18">
         <v>120</v>
       </c>
     </row>

</xml_diff>